<commit_message>
Fixed orientations in 12-12 teensy 4.1 arena fab files.
</commit_message>
<xml_diff>
--- a/development/arena_12-12/teensy4p1/teensy_arena_12-12_v0p1/production/version_0p1_r1/bom_cpl_wo_global_parts/CPL_JLCPCB_teensy_arena_12-12_v0p1_r1.xlsx
+++ b/development/arena_12-12/teensy4p1/teensy_arena_12-12_v0p1/production/version_0p1_r1/bom_cpl_wo_global_parts/CPL_JLCPCB_teensy_arena_12-12_v0p1_r1.xlsx
@@ -1473,10 +1473,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E426"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A313" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A108" activeCellId="0" sqref="A108"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A84" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G90" activeCellId="0" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3358,7 +3358,7 @@
         <v>6</v>
       </c>
       <c r="E110" s="2" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7353,8 +7353,9 @@
         <v>6</v>
       </c>
       <c r="E345" s="2" t="n">
-        <v>-90</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="F345" s="2"/>
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="2" t="s">
@@ -7370,7 +7371,7 @@
         <v>6</v>
       </c>
       <c r="E346" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7387,7 +7388,7 @@
         <v>6</v>
       </c>
       <c r="E347" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7404,7 +7405,7 @@
         <v>6</v>
       </c>
       <c r="E348" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7421,7 +7422,7 @@
         <v>6</v>
       </c>
       <c r="E349" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7438,7 +7439,7 @@
         <v>6</v>
       </c>
       <c r="E350" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7455,7 +7456,7 @@
         <v>6</v>
       </c>
       <c r="E351" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7472,7 +7473,7 @@
         <v>6</v>
       </c>
       <c r="E352" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7489,7 +7490,7 @@
         <v>6</v>
       </c>
       <c r="E353" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7506,7 +7507,7 @@
         <v>6</v>
       </c>
       <c r="E354" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7523,7 +7524,7 @@
         <v>6</v>
       </c>
       <c r="E355" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7540,7 +7541,7 @@
         <v>6</v>
       </c>
       <c r="E356" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7557,7 +7558,7 @@
         <v>6</v>
       </c>
       <c r="E357" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7574,7 +7575,7 @@
         <v>6</v>
       </c>
       <c r="E358" s="2" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7591,7 +7592,7 @@
         <v>6</v>
       </c>
       <c r="E359" s="2" t="n">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7608,7 +7609,7 @@
         <v>6</v>
       </c>
       <c r="E360" s="2" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7625,7 +7626,7 @@
         <v>6</v>
       </c>
       <c r="E361" s="2" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7642,7 +7643,7 @@
         <v>6</v>
       </c>
       <c r="E362" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7659,7 +7660,7 @@
         <v>6</v>
       </c>
       <c r="E363" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7676,7 +7677,7 @@
         <v>6</v>
       </c>
       <c r="E364" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7693,7 +7694,7 @@
         <v>6</v>
       </c>
       <c r="E365" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7710,7 +7711,7 @@
         <v>6</v>
       </c>
       <c r="E366" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7727,7 +7728,7 @@
         <v>6</v>
       </c>
       <c r="E367" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7744,7 +7745,7 @@
         <v>6</v>
       </c>
       <c r="E368" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7761,7 +7762,7 @@
         <v>6</v>
       </c>
       <c r="E369" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7778,7 +7779,7 @@
         <v>6</v>
       </c>
       <c r="E370" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7795,7 +7796,7 @@
         <v>6</v>
       </c>
       <c r="E371" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7812,7 +7813,7 @@
         <v>6</v>
       </c>
       <c r="E372" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7829,7 +7830,7 @@
         <v>6</v>
       </c>
       <c r="E373" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7846,7 +7847,7 @@
         <v>6</v>
       </c>
       <c r="E374" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7863,7 +7864,7 @@
         <v>6</v>
       </c>
       <c r="E375" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7880,7 +7881,7 @@
         <v>6</v>
       </c>
       <c r="E376" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7897,7 +7898,7 @@
         <v>6</v>
       </c>
       <c r="E377" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7914,7 +7915,7 @@
         <v>6</v>
       </c>
       <c r="E378" s="2" t="n">
-        <v>-90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7931,7 +7932,7 @@
         <v>6</v>
       </c>
       <c r="E379" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7948,7 +7949,7 @@
         <v>6</v>
       </c>
       <c r="E380" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7965,7 +7966,7 @@
         <v>6</v>
       </c>
       <c r="E381" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7982,7 +7983,7 @@
         <v>6</v>
       </c>
       <c r="E382" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7999,7 +8000,7 @@
         <v>6</v>
       </c>
       <c r="E383" s="2" t="n">
-        <v>-150</v>
+        <v>-240</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8016,7 +8017,7 @@
         <v>6</v>
       </c>
       <c r="E384" s="2" t="n">
-        <v>-150</v>
+        <v>-240</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8033,7 +8034,7 @@
         <v>6</v>
       </c>
       <c r="E385" s="2" t="n">
-        <v>-150</v>
+        <v>-240</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8050,7 +8051,7 @@
         <v>6</v>
       </c>
       <c r="E386" s="2" t="n">
-        <v>-150</v>
+        <v>-240</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8067,7 +8068,7 @@
         <v>6</v>
       </c>
       <c r="E387" s="2" t="n">
-        <v>-120</v>
+        <v>-210</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8084,7 +8085,7 @@
         <v>6</v>
       </c>
       <c r="E388" s="2" t="n">
-        <v>-120</v>
+        <v>-210</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8101,7 +8102,7 @@
         <v>6</v>
       </c>
       <c r="E389" s="2" t="n">
-        <v>-120</v>
+        <v>-210</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8118,7 +8119,7 @@
         <v>6</v>
       </c>
       <c r="E390" s="2" t="n">
-        <v>-120</v>
+        <v>-210</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8135,7 +8136,7 @@
         <v>6</v>
       </c>
       <c r="E391" s="2" t="n">
-        <v>-90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8152,7 +8153,7 @@
         <v>6</v>
       </c>
       <c r="E392" s="2" t="n">
-        <v>-90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8169,7 +8170,7 @@
         <v>6</v>
       </c>
       <c r="E393" s="2" t="n">
-        <v>-90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8186,7 +8187,7 @@
         <v>6</v>
       </c>
       <c r="E394" s="2" t="n">
-        <v>-90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8203,7 +8204,7 @@
         <v>6</v>
       </c>
       <c r="E395" s="2" t="n">
-        <v>-60</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8220,7 +8221,7 @@
         <v>6</v>
       </c>
       <c r="E396" s="2" t="n">
-        <v>-60</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8237,7 +8238,7 @@
         <v>6</v>
       </c>
       <c r="E397" s="2" t="n">
-        <v>-60</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8254,7 +8255,7 @@
         <v>6</v>
       </c>
       <c r="E398" s="2" t="n">
-        <v>-60</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8271,7 +8272,7 @@
         <v>6</v>
       </c>
       <c r="E399" s="2" t="n">
-        <v>-30</v>
+        <v>-120</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8288,7 +8289,7 @@
         <v>6</v>
       </c>
       <c r="E400" s="2" t="n">
-        <v>-30</v>
+        <v>-120</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8305,7 +8306,7 @@
         <v>6</v>
       </c>
       <c r="E401" s="2" t="n">
-        <v>-30</v>
+        <v>-120</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8322,7 +8323,7 @@
         <v>6</v>
       </c>
       <c r="E402" s="2" t="n">
-        <v>-30</v>
+        <v>-120</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8339,7 +8340,7 @@
         <v>6</v>
       </c>
       <c r="E403" s="2" t="n">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8356,7 +8357,7 @@
         <v>6</v>
       </c>
       <c r="E404" s="2" t="n">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8373,7 +8374,7 @@
         <v>6</v>
       </c>
       <c r="E405" s="2" t="n">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8390,7 +8391,7 @@
         <v>6</v>
       </c>
       <c r="E406" s="2" t="n">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8407,7 +8408,7 @@
         <v>6</v>
       </c>
       <c r="E407" s="2" t="n">
-        <v>30</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8424,7 +8425,7 @@
         <v>6</v>
       </c>
       <c r="E408" s="2" t="n">
-        <v>30</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8441,7 +8442,7 @@
         <v>6</v>
       </c>
       <c r="E409" s="2" t="n">
-        <v>30</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8458,7 +8459,7 @@
         <v>6</v>
       </c>
       <c r="E410" s="2" t="n">
-        <v>30</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8475,7 +8476,7 @@
         <v>6</v>
       </c>
       <c r="E411" s="2" t="n">
-        <v>60</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8492,7 +8493,7 @@
         <v>6</v>
       </c>
       <c r="E412" s="2" t="n">
-        <v>60</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8509,7 +8510,7 @@
         <v>6</v>
       </c>
       <c r="E413" s="2" t="n">
-        <v>60</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8526,7 +8527,7 @@
         <v>6</v>
       </c>
       <c r="E414" s="2" t="n">
-        <v>60</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8543,7 +8544,7 @@
         <v>6</v>
       </c>
       <c r="E415" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8560,7 +8561,7 @@
         <v>6</v>
       </c>
       <c r="E416" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8577,7 +8578,7 @@
         <v>6</v>
       </c>
       <c r="E417" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8594,7 +8595,7 @@
         <v>6</v>
       </c>
       <c r="E418" s="2" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8611,7 +8612,7 @@
         <v>6</v>
       </c>
       <c r="E419" s="2" t="n">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8628,7 +8629,7 @@
         <v>6</v>
       </c>
       <c r="E420" s="2" t="n">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8645,7 +8646,7 @@
         <v>6</v>
       </c>
       <c r="E421" s="2" t="n">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8662,7 +8663,7 @@
         <v>6</v>
       </c>
       <c r="E422" s="2" t="n">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8679,7 +8680,7 @@
         <v>6</v>
       </c>
       <c r="E423" s="2" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8696,7 +8697,7 @@
         <v>6</v>
       </c>
       <c r="E424" s="2" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8713,7 +8714,7 @@
         <v>6</v>
       </c>
       <c r="E425" s="2" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8730,9 +8731,24 @@
         <v>6</v>
       </c>
       <c r="E426" s="2" t="n">
-        <v>150</v>
-      </c>
-    </row>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>